<commit_message>
correção menos / menos para menas / menos
</commit_message>
<xml_diff>
--- a/data/como_se_escreve.xlsx
+++ b/data/como_se_escreve.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\farol_sign\conteudo.farolsign.com.br\servicos\como_se_escreve\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\como_se_escreve\www\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1449,10 +1449,10 @@
     <t>Namorar com alguém / Namorar alguém</t>
   </si>
   <si>
-    <t>Menos / Menos</t>
-  </si>
-  <si>
     <t>A cerca de / Acerca de</t>
+  </si>
+  <si>
+    <t>Menas / Menos</t>
   </si>
 </sst>
 </file>
@@ -2043,16 +2043,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -3569,7 +3569,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>418</v>
@@ -3583,7 +3583,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>421</v>

</xml_diff>